<commit_message>
Escaleta y documentos ajustados
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/SolicitudGrafica_CN_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/SolicitudGrafica_CN_08_01_CO.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="162">
   <si>
     <t>Fecha:</t>
   </si>
@@ -552,6 +552,9 @@
   <si>
     <t>Corte transversal de la médula espinal conectada con neurona sensitiva y neurona motora</t>
   </si>
+  <si>
+    <t>Silueta de un hombre bebiendo detrás de varias botellas</t>
+  </si>
 </sst>
 </file>
 
@@ -560,7 +563,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -708,6 +711,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1257,7 +1266,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1467,6 +1476,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1551,14 +1568,7 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2308,9 +2318,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2348,14 +2358,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="F2" s="79" t="s">
+      <c r="D2" s="91"/>
+      <c r="F2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="80"/>
+      <c r="G2" s="84"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
       <c r="J2" s="16"/>
@@ -2365,14 +2375,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="92">
         <v>8</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="F3" s="81">
+      <c r="D3" s="93"/>
+      <c r="F3" s="85">
         <v>42099</v>
       </c>
-      <c r="G3" s="82"/>
+      <c r="G3" s="86"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
       <c r="J3" s="16"/>
@@ -2382,10 +2392,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="5"/>
       <c r="F4" s="54" t="s">
         <v>55</v>
@@ -2403,10 +2413,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="91"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="5"/>
       <c r="F5" s="52" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2455,12 +2465,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="89"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2509,7 +2519,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="80" t="s">
         <v>149</v>
       </c>
       <c r="C10" s="27" t="str">
@@ -2538,7 +2548,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J10" s="112" t="s">
+      <c r="J10" s="81" t="s">
         <v>152</v>
       </c>
       <c r="K10" s="19"/>
@@ -2548,7 +2558,7 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="80" t="s">
         <v>153</v>
       </c>
       <c r="C11" s="27" t="str">
@@ -2577,7 +2587,7 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="113" t="s">
+      <c r="J11" s="82" t="s">
         <v>154</v>
       </c>
       <c r="K11" s="15"/>
@@ -2587,7 +2597,7 @@
         <f t="shared" ref="A12:A30" si="3">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="80" t="s">
         <v>155</v>
       </c>
       <c r="C12" s="27" t="str">
@@ -2616,7 +2626,7 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="113" t="s">
+      <c r="J12" s="82" t="s">
         <v>156</v>
       </c>
       <c r="K12" s="19"/>
@@ -2626,7 +2636,7 @@
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="79" t="s">
         <v>157</v>
       </c>
       <c r="C13" s="27" t="str">
@@ -2655,7 +2665,7 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="110" t="s">
+      <c r="J13" s="79" t="s">
         <v>158</v>
       </c>
       <c r="K13" s="19"/>
@@ -2665,7 +2675,7 @@
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="79" t="s">
         <v>159</v>
       </c>
       <c r="C14" s="27" t="str">
@@ -2694,40 +2704,48 @@
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J14" s="110" t="s">
+      <c r="J14" s="79" t="s">
         <v>160</v>
       </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B15" s="28"/>
+        <v>IMG06</v>
+      </c>
+      <c r="B15" s="114">
+        <v>267910670</v>
+      </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+        <v>Cuaderno de Estudio</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>CN_08_01_CO_IMG06_small</v>
       </c>
       <c r="G15" s="14" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>526 x 370 px</v>
       </c>
       <c r="H15" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>CN_08_01_CO_IMG06_zoom</v>
       </c>
       <c r="I15" s="14" t="str">
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J15" s="21"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J15" s="79" t="s">
+        <v>161</v>
+      </c>
       <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
@@ -5204,25 +5222,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="100"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="46"/>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="98"/>
-      <c r="E2" s="99"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="103"/>
       <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -5230,11 +5248,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="46"/>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="105"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="109"/>
       <c r="F3" s="47"/>
       <c r="H3" s="37" t="s">
         <v>18</v>
@@ -5285,11 +5303,11 @@
       <c r="C5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="106" t="str">
+      <c r="D5" s="110" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="107"/>
+      <c r="E5" s="111"/>
       <c r="F5" s="47"/>
       <c r="H5" s="37" t="s">
         <v>22</v>
@@ -5334,12 +5352,12 @@
       <c r="C7" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="92" t="str">
+      <c r="D7" s="96" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="93"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="97"/>
       <c r="H7" s="37" t="s">
         <v>24</v>
       </c>
@@ -5433,14 +5451,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="96"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="100"/>
       <c r="I13" s="37" t="s">
         <v>33</v>
       </c>
@@ -5473,12 +5491,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="46"/>
-      <c r="C15" s="97" t="s">
+      <c r="C15" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="99"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="103"/>
       <c r="J15" s="37">
         <v>12</v>
       </c>
@@ -5518,12 +5536,12 @@
       <c r="C17" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="100" t="str">
+      <c r="D17" s="104" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="106"/>
       <c r="J17" s="37">
         <v>14</v>
       </c>
@@ -5539,12 +5557,12 @@
       <c r="C18" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="92" t="str">
+      <c r="D18" s="96" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="93"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="97"/>
       <c r="J18" s="37">
         <v>15</v>
       </c>
@@ -5936,41 +5954,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="112" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
+      <c r="A2" s="112"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="56" t="s">
         <v>65</v>
       </c>

</xml_diff>